<commit_message>
atualização atividades aula 08
</commit_message>
<xml_diff>
--- a/aula08/normalizacao.xlsx
+++ b/aula08/normalizacao.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno.tarde\Desktop\banco_dados_senai\aula08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CF1D667-7556-45B7-85AB-FEC0F8FD1C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4549C76-252E-451E-AB3A-F391AD9CFDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{1FD3EB37-9393-414E-8F96-E47B666944FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{1FD3EB37-9393-414E-8F96-E47B666944FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Exemplo 1FN" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,12 @@
     <sheet name="atividade1" sheetId="4" r:id="rId4"/>
     <sheet name="atividade2" sheetId="5" r:id="rId5"/>
     <sheet name="atividade3" sheetId="6" r:id="rId6"/>
+    <sheet name="atividade4" sheetId="7" r:id="rId7"/>
+    <sheet name="atividade5" sheetId="8" r:id="rId8"/>
+    <sheet name="atividade6" sheetId="9" r:id="rId9"/>
+    <sheet name="atividade7" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="108">
   <si>
     <t>Nome</t>
   </si>
@@ -277,6 +280,93 @@
   </si>
   <si>
     <t>ID_Professor</t>
+  </si>
+  <si>
+    <t>Telefone_Professor</t>
+  </si>
+  <si>
+    <t>História</t>
+  </si>
+  <si>
+    <t>Prof. Almeida</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Geografia</t>
+  </si>
+  <si>
+    <t>Prof. Mendes</t>
+  </si>
+  <si>
+    <t>tbl_aluno</t>
+  </si>
+  <si>
+    <t>ID_Telefone_Professor</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Endereço_Cliente</t>
+  </si>
+  <si>
+    <t>Rua B</t>
+  </si>
+  <si>
+    <t>1.50</t>
+  </si>
+  <si>
+    <t>tbl_aluno_professor_telefone</t>
+  </si>
+  <si>
+    <t>tbl_telefone_professor</t>
+  </si>
+  <si>
+    <t>ID_Cliente</t>
+  </si>
+  <si>
+    <t>ID_Endereço</t>
+  </si>
+  <si>
+    <t>ID_Projeto</t>
+  </si>
+  <si>
+    <t>Nome_Projeto</t>
+  </si>
+  <si>
+    <t>Responsável</t>
+  </si>
+  <si>
+    <t>Responsáveis_Contatos</t>
+  </si>
+  <si>
+    <t>Projeto A</t>
+  </si>
+  <si>
+    <t>[joao@email.com, joao2@email.com]</t>
+  </si>
+  <si>
+    <t>Projeto B</t>
+  </si>
+  <si>
+    <t>[maria@email.com]</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>8.0</t>
+  </si>
+  <si>
+    <t>9.0</t>
   </si>
 </sst>
 </file>
@@ -390,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -478,6 +568,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1854,6 +1947,80 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC90D73-A9D4-48A2-8801-1B51198F61EE}">
+  <dimension ref="B3:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0C69AD-B5B4-4321-A89B-CBC1CED70A19}">
   <dimension ref="A1"/>
@@ -1882,10 +2049,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B006783B-4D2C-4396-AFBA-DBE61F20D0B5}">
-  <dimension ref="B2:G49"/>
+  <dimension ref="B2:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:M24"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1896,25 +2063,17 @@
     <col min="4" max="4" width="28.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="10"/>
+    <col min="7" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>62</v>
       </c>
@@ -1922,9 +2081,8 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>33</v>
       </c>
@@ -1940,9 +2098,8 @@
       <c r="F4" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="12"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="15">
         <v>1</v>
       </c>
@@ -1958,9 +2115,8 @@
       <c r="F5" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="12"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="15">
         <v>2</v>
       </c>
@@ -1976,9 +2132,8 @@
       <c r="F6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="15">
         <v>3</v>
       </c>
@@ -1994,25 +2149,22 @@
       <c r="F7" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>61</v>
       </c>
@@ -2020,9 +2172,8 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
         <v>33</v>
       </c>
@@ -2036,9 +2187,8 @@
         <v>48</v>
       </c>
       <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="15">
         <v>1</v>
       </c>
@@ -2052,9 +2202,8 @@
         <v>1</v>
       </c>
       <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="15">
         <v>2</v>
       </c>
@@ -2068,9 +2217,8 @@
         <v>2</v>
       </c>
       <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="15">
         <v>3</v>
       </c>
@@ -2084,17 +2232,15 @@
         <v>1</v>
       </c>
       <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>65</v>
       </c>
@@ -2102,9 +2248,8 @@
       <c r="D16" s="20"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
         <v>66</v>
       </c>
@@ -2114,9 +2259,8 @@
       <c r="D17" s="14"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="23">
         <v>1</v>
       </c>
@@ -2125,24 +2269,21 @@
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>64</v>
       </c>
@@ -2150,9 +2291,8 @@
       <c r="D21" s="8"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="16" t="s">
         <v>48</v>
       </c>
@@ -2164,9 +2304,8 @@
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="24">
         <v>1</v>
       </c>
@@ -2178,9 +2317,8 @@
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="24">
         <v>2</v>
       </c>
@@ -2192,17 +2330,15 @@
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>64</v>
       </c>
@@ -2210,9 +2346,8 @@
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="13" t="s">
         <v>67</v>
       </c>
@@ -2222,9 +2357,8 @@
       <c r="D27" s="14"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="26">
         <v>1</v>
       </c>
@@ -2233,9 +2367,8 @@
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="26">
         <v>2</v>
       </c>
@@ -2244,17 +2377,15 @@
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
         <v>68</v>
       </c>
@@ -2262,9 +2393,8 @@
       <c r="D31" s="19"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="13" t="s">
         <v>69</v>
       </c>
@@ -2276,9 +2406,8 @@
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="17">
         <v>1</v>
       </c>
@@ -2290,9 +2419,8 @@
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="17">
         <v>2</v>
       </c>
@@ -2304,127 +2432,111 @@
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2438,7 +2550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D524ABE-F05C-4D94-8ECD-8EFF92F97392}">
   <dimension ref="B2:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2747,8 +2859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B21AC60-D162-4817-96AC-6BFD27C371A8}">
   <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2972,4 +3084,468 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9536197-3A4E-4B02-8356-70349E2127C0}">
+  <dimension ref="B2:F27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="12"/>
+    <col min="2" max="2" width="26.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="15">
+        <v>2</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="15">
+        <v>3</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="15">
+        <v>1</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="15">
+        <v>2</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="15">
+        <v>2</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="15">
+        <v>1</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="15">
+        <v>2</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="29"/>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="15">
+        <v>1</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="15">
+        <v>2</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="15">
+        <v>3</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D31DA3-F807-4C9D-81BB-3FC4F78BBFD5}">
+  <dimension ref="B2:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="12"/>
+    <col min="2" max="2" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+      <c r="C4" s="30">
+        <v>45292</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="15">
+        <v>2</v>
+      </c>
+      <c r="C5" s="30">
+        <v>45293</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="15">
+        <v>3</v>
+      </c>
+      <c r="C6" s="30">
+        <v>45292</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FD1900-5198-4842-869B-BC1F7C2AD7A8}">
+  <dimension ref="B3:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
+        <v>2</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização atividades aula 08 normalização
</commit_message>
<xml_diff>
--- a/aula08/normalizacao.xlsx
+++ b/aula08/normalizacao.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno.tarde\Desktop\banco_dados_senai\aula08\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anderson51599526\Desktop\banco_dados_senai\aula08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4549C76-252E-451E-AB3A-F391AD9CFDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{1FD3EB37-9393-414E-8F96-E47B666944FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Exemplo 1FN" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
     <sheet name="atividade6" sheetId="9" r:id="rId9"/>
     <sheet name="atividade7" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="125">
   <si>
     <t>Nome</t>
   </si>
@@ -330,9 +329,6 @@
     <t>ID_Cliente</t>
   </si>
   <si>
-    <t>ID_Endereço</t>
-  </si>
-  <si>
     <t>ID_Projeto</t>
   </si>
   <si>
@@ -367,13 +363,67 @@
   </si>
   <si>
     <t>9.0</t>
+  </si>
+  <si>
+    <t>ID_Contato_Responsavel</t>
+  </si>
+  <si>
+    <t>Contato_Responsável</t>
+  </si>
+  <si>
+    <t>joao@email.com</t>
+  </si>
+  <si>
+    <t>maria@email.com</t>
+  </si>
+  <si>
+    <t>joao2@email.com</t>
+  </si>
+  <si>
+    <t>ID_Responsavel</t>
+  </si>
+  <si>
+    <t>tbl_contato_responsavel</t>
+  </si>
+  <si>
+    <t>tbl_projeto_reponsavel_contato</t>
+  </si>
+  <si>
+    <t>Nome_Responsavel</t>
+  </si>
+  <si>
+    <t>tbl_responsavel</t>
+  </si>
+  <si>
+    <t>tbl_projeto</t>
+  </si>
+  <si>
+    <t>ID_Nota</t>
+  </si>
+  <si>
+    <t>tbl_nota</t>
+  </si>
+  <si>
+    <t>ID_curso</t>
+  </si>
+  <si>
+    <t>tbl_aluno_curso_nota</t>
+  </si>
+  <si>
+    <t>tbl_contato_fornecedor</t>
+  </si>
+  <si>
+    <t>tbl_venda_cliente_produto</t>
+  </si>
+  <si>
+    <t>tbl_cliente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,6 +450,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -477,10 +535,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -572,8 +631,15 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="31">
@@ -591,7 +657,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -628,7 +693,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -667,7 +731,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -706,7 +769,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -745,7 +807,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -782,7 +843,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -807,7 +867,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1294,8 +1353,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB2B5789-992E-49A6-A1EE-350A30C3610B}" name="Tabela1" displayName="Tabela1" ref="B2:F4" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="B2:F4" xr:uid="{DB2B5789-992E-49A6-A1EE-350A30C3610B}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B2:F4" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="B2:F4">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1303,65 +1362,65 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{07966C3F-0BE6-47D1-8030-2809DCAE5439}" name="Nome" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{29B74722-7E8A-4392-9C32-E9E9218B4F62}" name="Telefone" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{FB01CFE0-DF8F-4830-A009-C36A700A49FF}" name="Logradouro" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{E86750F4-F8C0-49BD-BC9C-D8498BDC0A4B}" name="Cidade" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{E1BBEFB0-8A3B-4D04-8319-B17B9E38D6C2}" name="Estado" dataDxfId="24"/>
+    <tableColumn id="1" name="Nome" dataDxfId="28"/>
+    <tableColumn id="2" name="Telefone" dataDxfId="27"/>
+    <tableColumn id="3" name="Logradouro" dataDxfId="26"/>
+    <tableColumn id="4" name="Cidade" dataDxfId="25"/>
+    <tableColumn id="5" name="Estado" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{391956B9-F3C3-412E-9BAF-A92BD1F42D2D}" name="Tabela2" displayName="Tabela2" ref="B8:C10" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="B8:C10" xr:uid="{391956B9-F3C3-412E-9BAF-A92BD1F42D2D}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B8:C10" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="B8:C10">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C814A258-6E82-4FD6-9ABB-437EEB7AC944}" name="id_tbl_estudante" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{B3C1F558-9A01-46A3-9F0F-E558AF434192}" name="Nome" dataDxfId="20"/>
+    <tableColumn id="1" name="id_tbl_estudante" dataDxfId="21"/>
+    <tableColumn id="2" name="Nome" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2B56137-F9FF-44A5-993A-6ED83322B78D}" name="Tabela3" displayName="Tabela3" ref="E8:H13" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="E8:H13" xr:uid="{A2B56137-F9FF-44A5-993A-6ED83322B78D}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="E8:H13" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="E8:H13">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E845711A-3ACE-44D9-BB19-0858DA5EF604}" name="id_tbl_telefone" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{8B84F9C9-20F1-4505-BD38-D52AC9BFDADA}" name="telefoneq" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{B5603ADA-875C-441D-B4ED-828D431174F7}" name="id_tbl_estudante" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{B535BBAA-BF8D-4B2D-A4A9-BF6E9912A269}" name="Tipo" dataDxfId="14"/>
+    <tableColumn id="1" name="id_tbl_telefone" dataDxfId="17"/>
+    <tableColumn id="2" name="telefoneq" dataDxfId="16"/>
+    <tableColumn id="3" name="id_tbl_estudante" dataDxfId="15"/>
+    <tableColumn id="4" name="Tipo" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{34AAA063-53DE-46D4-90B0-E254EC5E4E91}" name="Tabela4" displayName="Tabela4" ref="B18:F22" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="B18:F22" xr:uid="{34AAA063-53DE-46D4-90B0-E254EC5E4E91}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="B18:F22" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="B18:F22"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{76AE81C3-BF8C-4973-B10C-4375396756A4}" name="ID_Pedido" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{3D90907B-D607-4FE6-8A7F-F704BE3072C9}" name="Nome_Cliente" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{330903F9-2C07-4A0C-A377-16041A390674}" name="Produtos" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{1BAE09D2-E5AD-4C41-BA92-30611C033DF5}" name="Endereço" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{EA893BF5-84F9-418C-A18C-0AD4BFBAF121}" name="Telefone" dataDxfId="7"/>
+    <tableColumn id="1" name="ID_Pedido" dataDxfId="11"/>
+    <tableColumn id="2" name="Nome_Cliente" dataDxfId="10"/>
+    <tableColumn id="3" name="Produtos" dataDxfId="9"/>
+    <tableColumn id="4" name="Endereço" dataDxfId="8"/>
+    <tableColumn id="5" name="Telefone" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8F133F3E-6123-4617-BC51-50442FC356C4}" name="Tabela5" displayName="Tabela5" ref="B4:F7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="B4:F7" xr:uid="{8F133F3E-6123-4617-BC51-50442FC356C4}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="B4:F7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="B4:F7">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1369,11 +1428,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{51D6EE4F-9CF9-4E3D-8BF5-7865CEAAD7BE}" name="ID_Produto" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{15D0F13F-8EAD-4265-A072-2B5039B6C0F4}" name="Nome_Produto" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{563DB4A6-810D-49A9-A50C-953DA3C041BB}" name="Categoria" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{D7ACA48C-5366-451A-B76D-11B67C96C0F3}" name="Fornecedor" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{8D1BE297-FF79-436B-B220-51500073AA46}" name="Telefone_Fornecedor" dataDxfId="0"/>
+    <tableColumn id="1" name="ID_Produto" dataDxfId="4"/>
+    <tableColumn id="2" name="Nome_Produto" dataDxfId="3"/>
+    <tableColumn id="3" name="Categoria" dataDxfId="2"/>
+    <tableColumn id="4" name="Fornecedor" dataDxfId="1"/>
+    <tableColumn id="5" name="Telefone_Fornecedor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1675,27 +1734,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29AE32D3-560F-4B94-98A4-F887708B28A3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="18.26953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1704,7 +1763,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1721,7 +1780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1738,7 +1797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1755,11 +1814,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
@@ -1771,7 +1830,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
@@ -1791,7 +1850,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="6">
         <v>1</v>
       </c>
@@ -1811,7 +1870,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="6">
         <v>2</v>
       </c>
@@ -1831,7 +1890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="E11" s="4">
         <v>3</v>
       </c>
@@ -1845,7 +1904,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="E12" s="4">
         <v>4</v>
       </c>
@@ -1859,7 +1918,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="E13" s="4">
         <v>5</v>
       </c>
@@ -1873,7 +1932,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
@@ -1882,7 +1941,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="4" t="s">
         <v>27</v>
       </c>
@@ -1899,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
         <v>31</v>
@@ -1908,7 +1967,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
         <v>5</v>
@@ -1917,7 +1976,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>31</v>
@@ -1926,7 +1985,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
         <v>15</v>
@@ -1948,72 +2007,178 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC90D73-A9D4-48A2-8801-1B51198F61EE}">
-  <dimension ref="B3:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="9.1796875" style="12"/>
+    <col min="2" max="2" width="10.6328125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.08984375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="12"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12" t="s">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="15">
+        <v>1</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D5" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="15">
+        <v>2</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E6" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="15">
+        <v>1</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="15">
+        <v>2</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="15">
+        <v>2</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="12">
-        <v>1</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="D16" s="15">
+        <v>1</v>
+      </c>
+      <c r="E16" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="15">
+        <v>3</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="12">
-        <v>2</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>107</v>
+      <c r="D17" s="15">
+        <v>2</v>
+      </c>
+      <c r="E17" s="15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2022,58 +2187,58 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0C69AD-B5B4-4321-A89B-CBC1CED70A19}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECCAA574-C9F9-402A-9030-8802EA55E868}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B006783B-4D2C-4396-AFBA-DBE61F20D0B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="9.1796875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="29.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>62</v>
       </c>
@@ -2082,7 +2247,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>33</v>
       </c>
@@ -2099,7 +2264,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="15">
         <v>1</v>
       </c>
@@ -2116,7 +2281,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="15">
         <v>2</v>
       </c>
@@ -2133,7 +2298,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="15">
         <v>3</v>
       </c>
@@ -2150,21 +2315,21 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="14"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
         <v>61</v>
       </c>
@@ -2173,7 +2338,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="13" t="s">
         <v>33</v>
       </c>
@@ -2188,7 +2353,7 @@
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="15">
         <v>1</v>
       </c>
@@ -2203,7 +2368,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="15">
         <v>2</v>
       </c>
@@ -2218,7 +2383,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="15">
         <v>3</v>
       </c>
@@ -2233,14 +2398,14 @@
       </c>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
         <v>65</v>
       </c>
@@ -2249,7 +2414,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="13" t="s">
         <v>66</v>
       </c>
@@ -2260,7 +2425,7 @@
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="23">
         <v>1</v>
       </c>
@@ -2270,20 +2435,20 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="8" t="s">
         <v>64</v>
       </c>
@@ -2292,7 +2457,7 @@
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="16" t="s">
         <v>48</v>
       </c>
@@ -2305,7 +2470,7 @@
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" s="24">
         <v>1</v>
       </c>
@@ -2318,7 +2483,7 @@
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="24">
         <v>2</v>
       </c>
@@ -2331,23 +2496,23 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="8" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" s="13" t="s">
         <v>67</v>
       </c>
@@ -2358,7 +2523,7 @@
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" s="26">
         <v>1</v>
       </c>
@@ -2368,7 +2533,7 @@
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" s="26">
         <v>2</v>
       </c>
@@ -2378,14 +2543,14 @@
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B31" s="8" t="s">
         <v>68</v>
       </c>
@@ -2394,7 +2559,7 @@
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B32" s="13" t="s">
         <v>69</v>
       </c>
@@ -2407,7 +2572,7 @@
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B33" s="17">
         <v>1</v>
       </c>
@@ -2420,7 +2585,7 @@
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B34" s="17">
         <v>2</v>
       </c>
@@ -2433,105 +2598,105 @@
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
@@ -2547,24 +2712,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D524ABE-F05C-4D94-8ECD-8EFF92F97392}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>70</v>
       </c>
@@ -2574,7 +2739,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="13" t="s">
         <v>46</v>
       </c>
@@ -2594,7 +2759,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B4" s="8">
         <v>1</v>
       </c>
@@ -2614,7 +2779,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5" s="8">
         <v>2</v>
       </c>
@@ -2634,7 +2799,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="8">
         <v>3</v>
       </c>
@@ -2654,7 +2819,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -2662,7 +2827,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
         <v>61</v>
       </c>
@@ -2672,7 +2837,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B9" s="13" t="s">
         <v>33</v>
       </c>
@@ -2686,7 +2851,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B10" s="8">
         <v>101</v>
       </c>
@@ -2700,7 +2865,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B11" s="8">
         <v>102</v>
       </c>
@@ -2714,7 +2879,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
@@ -2722,7 +2887,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -2730,7 +2895,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B14" s="8" t="s">
         <v>64</v>
       </c>
@@ -2740,7 +2905,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B15" s="13" t="s">
         <v>48</v>
       </c>
@@ -2752,7 +2917,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B16" s="8">
         <v>1</v>
       </c>
@@ -2764,7 +2929,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B17" s="8">
         <v>2</v>
       </c>
@@ -2776,7 +2941,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
@@ -2784,7 +2949,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
         <v>73</v>
       </c>
@@ -2794,7 +2959,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B20" s="13" t="s">
         <v>46</v>
       </c>
@@ -2808,7 +2973,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B21" s="8">
         <v>1</v>
       </c>
@@ -2822,7 +2987,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B22" s="8">
         <v>2</v>
       </c>
@@ -2836,7 +3001,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B23" s="8">
         <v>3</v>
       </c>
@@ -2856,24 +3021,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B21AC60-D162-4817-96AC-6BFD27C371A8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="27"/>
-    <col min="2" max="2" width="15.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="27"/>
+    <col min="2" max="2" width="15.7265625" style="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" style="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="27"/>
+    <col min="6" max="16384" width="9.1796875" style="27"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" s="21" t="s">
         <v>77</v>
       </c>
@@ -2881,7 +3046,7 @@
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
     </row>
-    <row r="3" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" s="13" t="s">
         <v>52</v>
       </c>
@@ -2895,7 +3060,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" s="15">
         <v>1</v>
       </c>
@@ -2909,7 +3074,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="15">
         <v>2</v>
       </c>
@@ -2923,7 +3088,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" s="15">
         <v>3</v>
       </c>
@@ -2937,14 +3102,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" s="21" t="s">
         <v>75</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="29"/>
     </row>
-    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" s="13" t="s">
         <v>74</v>
       </c>
@@ -2953,7 +3118,7 @@
       </c>
       <c r="D9" s="14"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" s="28">
         <v>1</v>
       </c>
@@ -2962,7 +3127,7 @@
       </c>
       <c r="D10" s="12"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="28">
         <v>2</v>
       </c>
@@ -2971,17 +3136,17 @@
       </c>
       <c r="D11" s="12"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="21" t="s">
         <v>76</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
     </row>
-    <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="13" t="s">
         <v>78</v>
       </c>
@@ -2992,7 +3157,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="28">
         <v>1</v>
       </c>
@@ -3003,7 +3168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="28">
         <v>2</v>
       </c>
@@ -3014,10 +3179,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C17" s="12"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="21" t="s">
         <v>75</v>
       </c>
@@ -3025,7 +3190,7 @@
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
     </row>
-    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="13" t="s">
         <v>52</v>
       </c>
@@ -3039,7 +3204,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="15">
         <v>1</v>
       </c>
@@ -3053,7 +3218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="15">
         <v>2</v>
       </c>
@@ -3067,7 +3232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="15">
         <v>3</v>
       </c>
@@ -3087,34 +3252,34 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9536197-3A4E-4B02-8356-70349E2127C0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="12"/>
-    <col min="2" max="2" width="26.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="12"/>
+    <col min="2" max="2" width="26.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="12"/>
+    <col min="6" max="6" width="23.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="12"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="13" t="s">
         <v>52</v>
       </c>
@@ -3131,7 +3296,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="15">
         <v>1</v>
       </c>
@@ -3148,7 +3313,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="15">
         <v>2</v>
       </c>
@@ -3165,7 +3330,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="15">
         <v>3</v>
       </c>
@@ -3182,14 +3347,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="13" t="s">
         <v>74</v>
       </c>
@@ -3200,7 +3365,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="15">
         <v>1</v>
       </c>
@@ -3211,7 +3376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="15">
         <v>2</v>
       </c>
@@ -3222,13 +3387,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="9"/>
-    </row>
-    <row r="14" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="13" t="s">
         <v>78</v>
       </c>
@@ -3236,7 +3401,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="15">
         <v>1</v>
       </c>
@@ -3244,7 +3409,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="15">
         <v>2</v>
       </c>
@@ -3252,14 +3417,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-    </row>
-    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="13" t="s">
         <v>86</v>
       </c>
@@ -3270,7 +3435,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="15">
         <v>1</v>
       </c>
@@ -3281,7 +3446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="15">
         <v>2</v>
       </c>
@@ -3292,7 +3457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="8" t="s">
         <v>85</v>
       </c>
@@ -3300,7 +3465,7 @@
       <c r="D23" s="8"/>
       <c r="E23" s="29"/>
     </row>
-    <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="13" t="s">
         <v>52</v>
       </c>
@@ -3312,7 +3477,7 @@
       </c>
       <c r="E24" s="14"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="15">
         <v>1</v>
       </c>
@@ -3323,7 +3488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="15">
         <v>2</v>
       </c>
@@ -3334,7 +3499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="15">
         <v>3</v>
       </c>
@@ -3352,34 +3517,35 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D31DA3-F807-4C9D-81BB-3FC4F78BBFD5}">
-  <dimension ref="B2:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="12"/>
-    <col min="2" max="2" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="12"/>
+    <col min="2" max="2" width="14.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.54296875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="12"/>
+    <col min="6" max="6" width="18.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="12"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="9"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B2" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B3" s="13" t="s">
         <v>46</v>
       </c>
@@ -3399,7 +3565,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="15">
         <v>1</v>
       </c>
@@ -3419,7 +3585,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="15">
         <v>2</v>
       </c>
@@ -3439,7 +3605,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" s="15">
         <v>3</v>
       </c>
@@ -3459,30 +3625,121 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B8" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B9" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B10" s="12">
+        <v>1</v>
+      </c>
       <c r="C10" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D10" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B11" s="12">
+        <v>2</v>
+      </c>
       <c r="C11" s="12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>2</v>
+      <c r="D11" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B15" s="15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B16" s="15">
+        <v>2</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="15">
+        <v>2</v>
+      </c>
+      <c r="F16" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="15">
+        <v>3</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="15">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3491,61 +3748,201 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FD1900-5198-4842-869B-BC1F7C2AD7A8}">
-  <dimension ref="B3:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="9.1796875" style="12"/>
+    <col min="2" max="2" width="27.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.08984375" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.90625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.7265625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="12"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="12" t="s">
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="D4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="12" t="s">
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="15">
+        <v>2</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="15">
+        <v>1</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="15">
+        <v>2</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="15">
+        <v>1</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="12" t="s">
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="15">
+        <v>2</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="15">
+        <v>1</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="15">
+        <v>2</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="12">
-        <v>2</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>103</v>
+      <c r="D21" s="15">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1"/>
+    <hyperlink ref="C10" r:id="rId2"/>
+    <hyperlink ref="C11" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>